<commit_message>
Zc VerifPlan: added exception handling for push/pop
Signed-off-by: Marton Teilgard <mateilga@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/Zc/RV32Zc_Extension_Instructions.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/Zc/RV32Zc_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif\cv32e40s\docs\VerifPlans\Simulation\Zc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41137F5D-0CF9-4219-A96B-FD07AC8E8557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6648E5B-D6C2-4247-8A8E-8560D7D60846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-11040" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zc" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="114">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>Verify interrupts(maskable and non-maskable), debug and single stepping can not stop execution after the instruction has started to change state. Make sure external interrupts happen at all stages of execution. Expect atomic execution</t>
+  </si>
+  <si>
+    <t>Verify exception behaviour, partially completed state shall match ISS: when a multi-operation instruction is stopped by an exception, state can have changed. Verify against ISS.
+Note: 40s implementation follows the example sequence in the Zc spec. ISS's should match this. 
+Coverage note: cross between possible register lists and exception arriving between/at all sub-operations would be optimal</t>
+  </si>
+  <si>
+    <t>Verify exception behaviour, no following bus transaction: if a sub-operation triggers an exception, no further transaction shall arrive on the bus originating in the trapped instruction
+Note: this functionality is closely matched with items mentioned in other features of the 40s, such as PMP/PMA. Synchronize verification effort to avoid double work.</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -508,6 +517,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -515,13 +542,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,30 +926,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ128"/>
+  <dimension ref="A1:AMJ140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.5546875" style="1" customWidth="1"/>
     <col min="10" max="1023" width="17" style="1"/>
-    <col min="1024" max="1024" width="9.140625" style="1" customWidth="1"/>
+    <col min="1024" max="1024" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="30">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="28.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -957,8 +978,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A2" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -984,8 +1005,8 @@
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A3" s="22"/>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A3" s="28"/>
       <c r="B3" s="23"/>
       <c r="C3" s="19" t="s">
         <v>43</v>
@@ -1007,12 +1028,12 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A4" s="22"/>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A4" s="28"/>
       <c r="B4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="23" t="s">
@@ -1032,10 +1053,10 @@
       </c>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A5" s="22"/>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A5" s="28"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="20"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="23"/>
       <c r="E5" s="16" t="s">
         <v>95</v>
@@ -1051,13 +1072,13 @@
       </c>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A6" s="22"/>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A6" s="28"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="24" t="s">
         <v>71</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -1074,11 +1095,11 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A7" s="22"/>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A7" s="28"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="16" t="s">
         <v>95</v>
       </c>
@@ -1093,13 +1114,13 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A8" s="22"/>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A8" s="28"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -1116,11 +1137,11 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A9" s="22"/>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A9" s="28"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="16" t="s">
         <v>95</v>
       </c>
@@ -1135,13 +1156,13 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A10" s="22"/>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A10" s="28"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="24" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="16" t="s">
@@ -1158,11 +1179,11 @@
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A11" s="28"/>
       <c r="B11" s="23"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="16" t="s">
         <v>95</v>
       </c>
@@ -1177,13 +1198,13 @@
       </c>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A12" s="22"/>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A12" s="28"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="24" t="s">
         <v>74</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -1200,11 +1221,11 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A13" s="22"/>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A13" s="28"/>
       <c r="B13" s="23"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="16" t="s">
         <v>95</v>
       </c>
@@ -1219,8 +1240,8 @@
       </c>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A14" s="22"/>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A14" s="28"/>
       <c r="B14" s="23"/>
       <c r="C14" s="19" t="s">
         <v>50</v>
@@ -1242,8 +1263,8 @@
       </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A15" s="22"/>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A15" s="28"/>
       <c r="B15" s="23"/>
       <c r="C15" s="19" t="s">
         <v>51</v>
@@ -1265,8 +1286,8 @@
       </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A16" s="22"/>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A16" s="28"/>
       <c r="B16" s="23"/>
       <c r="C16" s="19" t="s">
         <v>52</v>
@@ -1288,8 +1309,8 @@
       </c>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A17" s="22"/>
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A17" s="28"/>
       <c r="B17" s="23"/>
       <c r="C17" s="19" t="s">
         <v>53</v>
@@ -1311,8 +1332,8 @@
       </c>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A18" s="28"/>
       <c r="B18" s="23"/>
       <c r="C18" s="19" t="s">
         <v>54</v>
@@ -1334,13 +1355,13 @@
       </c>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A19" s="22"/>
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A19" s="28"/>
       <c r="B19" s="23"/>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="24" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="16" t="s">
@@ -1357,11 +1378,11 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A20" s="22"/>
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A20" s="28"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="16" t="s">
         <v>98</v>
       </c>
@@ -1376,15 +1397,15 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A21" s="22"/>
+    <row r="21" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A21" s="28"/>
       <c r="B21" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="16" t="s">
@@ -1401,11 +1422,11 @@
       </c>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A22" s="22"/>
+    <row r="22" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A22" s="28"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="16" t="s">
         <v>95</v>
       </c>
@@ -1420,13 +1441,13 @@
       </c>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A23" s="22"/>
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A23" s="28"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="24" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -1443,11 +1464,11 @@
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A24" s="22"/>
+    <row r="24" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A24" s="28"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="16" t="s">
         <v>95</v>
       </c>
@@ -1462,13 +1483,13 @@
       </c>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A25" s="22"/>
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A25" s="28"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="24" t="s">
         <v>81</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -1485,11 +1506,11 @@
       </c>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A26" s="28"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="16" t="s">
         <v>95</v>
       </c>
@@ -1504,13 +1525,13 @@
       </c>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A27" s="22"/>
+    <row r="27" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A27" s="28"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -1527,11 +1548,11 @@
       </c>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A28" s="28"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="16" t="s">
         <v>95</v>
       </c>
@@ -1546,13 +1567,13 @@
       </c>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A29" s="22"/>
+    <row r="29" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A29" s="28"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="24" t="s">
         <v>73</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -1569,11 +1590,11 @@
       </c>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A30" s="22"/>
+    <row r="30" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A30" s="28"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="16" t="s">
         <v>95</v>
       </c>
@@ -1588,13 +1609,13 @@
       </c>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A31" s="22"/>
+    <row r="31" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A31" s="28"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="24" t="s">
         <v>74</v>
       </c>
       <c r="E31" s="16" t="s">
@@ -1611,11 +1632,11 @@
       </c>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A32" s="22"/>
+    <row r="32" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A32" s="28"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="16" t="s">
         <v>95</v>
       </c>
@@ -1631,11 +1652,11 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A33" s="22"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="25" t="s">
@@ -1655,10 +1676,10 @@
       </c>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A34" s="22"/>
+    <row r="34" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A34" s="28"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="20"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="25"/>
       <c r="E34" s="16" t="s">
         <v>105</v>
@@ -1674,10 +1695,10 @@
       </c>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A35" s="22"/>
+    <row r="35" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A35" s="28"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="20"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="25"/>
       <c r="E35" s="19" t="s">
         <v>111</v>
@@ -1693,287 +1714,273 @@
       </c>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A36" s="22"/>
+    <row r="36" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A36" s="28"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A37" s="28"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A38" s="28"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D38" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E38" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="16" t="s">
+      <c r="F38" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A39" s="28"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="19" t="s">
+      <c r="F39" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A40" s="28"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" s="19" t="s">
+      <c r="F40" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H40" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="20" t="s">
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A41" s="28"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A42" s="28"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A43" s="28"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D43" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="16" t="s">
+      <c r="F43" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A44" s="28"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A41" s="22"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="19" t="s">
+      <c r="F44" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A45" s="28"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" s="19" t="s">
+      <c r="F45" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H45" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="20" t="s">
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A46" s="28"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A47" s="28"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="12"/>
+    </row>
+    <row r="48" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A48" s="28"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D48" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E48" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="16" t="s">
+      <c r="F48" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A49" s="28"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A45" s="22"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A46" s="22"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F46" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A47" s="22"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="12"/>
-    </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A48" s="22"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="12"/>
-    </row>
-    <row r="49" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A49" s="22"/>
-      <c r="B49" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>99</v>
-      </c>
       <c r="F49" s="19" t="s">
         <v>92</v>
       </c>
@@ -1985,10 +1992,10 @@
       </c>
       <c r="I49" s="12"/>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A50" s="22"/>
+    <row r="50" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A50" s="28"/>
       <c r="B50" s="23"/>
-      <c r="C50" s="20"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="24"/>
       <c r="E50" s="19" t="s">
         <v>111</v>
@@ -2004,251 +2011,361 @@
       </c>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A51" s="22"/>
+    <row r="51" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A51" s="28"/>
       <c r="B51" s="23"/>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A52" s="28"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" s="12"/>
+    </row>
+    <row r="53" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A53" s="28"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="12"/>
+    </row>
+    <row r="54" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A54" s="28"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A55" s="28"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A56" s="28"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="57" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A57" s="28"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" s="12"/>
+    </row>
+    <row r="58" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A58" s="28"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A59" s="28"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A60" s="28"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="12"/>
+    </row>
+    <row r="61" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A61" s="28"/>
+      <c r="B61" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" s="12"/>
+    </row>
+    <row r="62" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A62" s="28"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" s="12"/>
+    </row>
+    <row r="63" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A63" s="28"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E63" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" s="12"/>
-    </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" ht="85.5">
-      <c r="A52" s="22"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="19" t="s">
+      <c r="F63" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="12"/>
+    </row>
+    <row r="64" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A64" s="28"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G52" s="19" t="s">
+      <c r="F64" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H52" s="18" t="s">
+      <c r="H64" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="12"/>
-    </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" ht="42.75">
-      <c r="A53" s="22"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="20" t="s">
+      <c r="I64" s="12"/>
+    </row>
+    <row r="65" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A65" s="28"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D65" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E65" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="F53" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="19" t="s">
+      <c r="F65" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H65" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="12"/>
-    </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A54" s="22"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="19" t="s">
+      <c r="I65" s="12"/>
+    </row>
+    <row r="66" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A66" s="28"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F54" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G54" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I54" s="12"/>
-    </row>
-    <row r="55" spans="1:9" s="3" customFormat="1" ht="28.5">
-      <c r="A55" s="22"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="19" t="s">
+      <c r="F66" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="12"/>
+    </row>
+    <row r="67" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A67" s="28"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F55" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" s="19" t="s">
+      <c r="F67" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="12"/>
-    </row>
-    <row r="56" spans="1:9" s="3" customFormat="1">
-      <c r="A56" s="4"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-    </row>
-    <row r="57" spans="1:9" s="3" customFormat="1">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="1:9" s="3" customFormat="1">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="1:9" s="3" customFormat="1">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-    </row>
-    <row r="60" spans="1:9" s="3" customFormat="1">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-    </row>
-    <row r="61" spans="1:9" s="3" customFormat="1">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-    </row>
-    <row r="62" spans="1:9" s="3" customFormat="1">
-      <c r="A62" s="4"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-    </row>
-    <row r="63" spans="1:9" s="3" customFormat="1">
-      <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-    </row>
-    <row r="64" spans="1:9" s="3" customFormat="1">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-    </row>
-    <row r="65" spans="1:9" s="3" customFormat="1">
-      <c r="A65" s="4"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-    </row>
-    <row r="66" spans="1:9" s="3" customFormat="1">
-      <c r="A66" s="4"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-    </row>
-    <row r="67" spans="1:9" s="3" customFormat="1">
-      <c r="A67" s="4"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
+      <c r="H67" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" s="12"/>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1">
       <c r="A68" s="4"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1">
       <c r="A69" s="4"/>
@@ -2478,8 +2595,8 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
-      <c r="H89" s="4"/>
-      <c r="I89" s="4"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
     </row>
     <row r="90" spans="1:9" s="3" customFormat="1">
       <c r="A90" s="4"/>
@@ -2489,8 +2606,8 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
     </row>
     <row r="91" spans="1:9" s="3" customFormat="1">
       <c r="A91" s="4"/>
@@ -2500,8 +2617,8 @@
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
     </row>
     <row r="92" spans="1:9" s="3" customFormat="1">
       <c r="A92" s="4"/>
@@ -2511,8 +2628,8 @@
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
     </row>
     <row r="93" spans="1:9" s="3" customFormat="1">
       <c r="A93" s="4"/>
@@ -2522,8 +2639,8 @@
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
     </row>
     <row r="94" spans="1:9" s="3" customFormat="1">
       <c r="A94" s="4"/>
@@ -2533,8 +2650,8 @@
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
     </row>
     <row r="95" spans="1:9" s="3" customFormat="1">
       <c r="A95" s="4"/>
@@ -2544,8 +2661,8 @@
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
     </row>
     <row r="96" spans="1:9" s="3" customFormat="1">
       <c r="A96" s="4"/>
@@ -2555,8 +2672,8 @@
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
     </row>
     <row r="97" spans="1:9" s="3" customFormat="1">
       <c r="A97" s="4"/>
@@ -2566,8 +2683,8 @@
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
     </row>
     <row r="98" spans="1:9" s="3" customFormat="1">
       <c r="A98" s="4"/>
@@ -2577,8 +2694,8 @@
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
     </row>
     <row r="99" spans="1:9" s="3" customFormat="1">
       <c r="A99" s="4"/>
@@ -2588,8 +2705,8 @@
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
     </row>
     <row r="100" spans="1:9" s="3" customFormat="1">
       <c r="A100" s="4"/>
@@ -2599,8 +2716,8 @@
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
     </row>
     <row r="101" spans="1:9" s="3" customFormat="1">
       <c r="A101" s="4"/>
@@ -2899,46 +3016,184 @@
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
     </row>
-    <row r="128" spans="1:9" s="6" customFormat="1">
-      <c r="A128" s="21" t="s">
+    <row r="128" spans="1:9" s="3" customFormat="1">
+      <c r="A128" s="4"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+    </row>
+    <row r="129" spans="1:9" s="3" customFormat="1">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+    </row>
+    <row r="130" spans="1:9" s="3" customFormat="1">
+      <c r="A130" s="4"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="4"/>
+    </row>
+    <row r="131" spans="1:9" s="3" customFormat="1">
+      <c r="A131" s="4"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+    </row>
+    <row r="132" spans="1:9" s="3" customFormat="1">
+      <c r="A132" s="4"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+    </row>
+    <row r="133" spans="1:9" s="3" customFormat="1">
+      <c r="A133" s="4"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+    </row>
+    <row r="134" spans="1:9" s="3" customFormat="1">
+      <c r="A134" s="4"/>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+    </row>
+    <row r="135" spans="1:9" s="3" customFormat="1">
+      <c r="A135" s="4"/>
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+    </row>
+    <row r="136" spans="1:9" s="3" customFormat="1">
+      <c r="A136" s="4"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="1:9" s="3" customFormat="1">
+      <c r="A137" s="4"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9" s="3" customFormat="1">
+      <c r="A138" s="4"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+    </row>
+    <row r="139" spans="1:9" s="3" customFormat="1">
+      <c r="A139" s="4"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="1:9" s="6" customFormat="1">
+      <c r="A140" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B128" s="21"/>
-      <c r="C128" s="21"/>
-      <c r="D128" s="21"/>
-      <c r="E128" s="21"/>
-      <c r="F128" s="21"/>
-      <c r="G128" s="21"/>
-      <c r="H128" s="21"/>
-      <c r="I128" s="21"/>
+      <c r="B140" s="27"/>
+      <c r="C140" s="27"/>
+      <c r="D140" s="27"/>
+      <c r="E140" s="27"/>
+      <c r="F140" s="27"/>
+      <c r="G140" s="27"/>
+      <c r="H140" s="27"/>
+      <c r="I140" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="B33:B48"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
+  <mergeCells count="59">
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A128:I128"/>
-    <mergeCell ref="A2:A55"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A140:I140"/>
+    <mergeCell ref="A2:A67"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B20"/>
     <mergeCell ref="B21:B32"/>
-    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B61:B67"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D8:D9"/>
@@ -2949,20 +3204,24 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="B33:B58"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C33:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2976,7 +3235,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H127</xm:sqref>
+          <xm:sqref>H2:H139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -2985,7 +3244,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G2:G127</xm:sqref>
+          <xm:sqref>G2:G139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -2994,7 +3253,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F127</xm:sqref>
+          <xm:sqref>F2:F139</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3010,11 +3269,11 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -3120,13 +3379,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" customWidth="1"/>
-    <col min="4" max="4" width="92.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="4" max="4" width="92.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">

</xml_diff>

<commit_message>
"Updated Zc vplan after internal review"
Signed-off-by: Marton Teilgard <mateilga@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/Zc/RV32Zc_Extension_Instructions.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/Zc/RV32Zc_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif\cv32e40s\docs\VerifPlans\Simulation\Zc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\localWork\openHW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6648E5B-D6C2-4247-8A8E-8560D7D60846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F7F552-E663-4ED9-98A8-5A2E6DEEAF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-11040" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="1680" windowWidth="28800" windowHeight="16680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zc" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,12 @@
     <sheet name="References" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="124">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -119,42 +115,12 @@
     <t>Git Hub Hash (if appropriate)</t>
   </si>
   <si>
-    <t>OBIv1.0</t>
-  </si>
-  <si>
-    <t>Open Bus Interface (OBI) Specification, v1.0, 3/5/2020</t>
-  </si>
-  <si>
-    <t>https://github.com/openhwgroup/core-v-docs/blob/master/cores/cv32e40p/OBI-v1.0.pdf</t>
-  </si>
-  <si>
-    <t>UM ac0641d</t>
-  </si>
-  <si>
-    <t>CV32E40P User Manual</t>
-  </si>
-  <si>
-    <t>https://github.com/openhwgroup/core-v-docs/tree/master/cores/cv32e40p/user_manual</t>
-  </si>
-  <si>
-    <t>ac0641d453715dd211c7674808d3ac08c64cc983</t>
-  </si>
-  <si>
     <t>Zca</t>
   </si>
   <si>
-    <t>Zcb</t>
-  </si>
-  <si>
-    <t>Zcmb</t>
-  </si>
-  <si>
     <t>Zcmp</t>
   </si>
   <si>
-    <t>Zcmt</t>
-  </si>
-  <si>
     <t>c.f*</t>
   </si>
   <si>
@@ -300,9 +266,6 @@
   </si>
   <si>
     <t>floating point load stores shall decode as illegal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that all variations of these instructions decode as illegal </t>
   </si>
   <si>
     <t>Check against ISS</t>
@@ -366,9 +329,6 @@
     <t>Zc* v0.70.5</t>
   </si>
   <si>
-    <t>csr stateen bit 2 controls user mode access, if bit is not set, cm.jt and cm.jalt should decode as illegal</t>
-  </si>
-  <si>
     <t>M_EXT=M_NONE shall result in c.mul decoding as an illegal instruction</t>
   </si>
   <si>
@@ -382,6 +342,82 @@
   <si>
     <t>Verify exception behaviour, no following bus transaction: if a sub-operation triggers an exception, no further transaction shall arrive on the bus originating in the trapped instruction
 Note: this functionality is closely matched with items mentioned in other features of the 40s, such as PMP/PMA. Synchronize verification effort to avoid double work.</t>
+  </si>
+  <si>
+    <t>OBIv1.4</t>
+  </si>
+  <si>
+    <t>Open Bus Interface (OBI) Specification, v1.4, 3/8/2022</t>
+  </si>
+  <si>
+    <t>https://github.com/openhwgroup/core-v-docs/blob/master/cores/obi/OBI-v1.4.pdf</t>
+  </si>
+  <si>
+    <t>4fdcf97be297201398f6abdd0bfca5e1e1d76440</t>
+  </si>
+  <si>
+    <t>UM 40205f</t>
+  </si>
+  <si>
+    <t>CV32E40S User Manual</t>
+  </si>
+  <si>
+    <t>https://docs.openhwgroup.org/projects/cv32e40s-user-manual/en/0.4.0/index.html</t>
+  </si>
+  <si>
+    <t>40205ff125fde4e8f0d3512b83170021fc8309f5</t>
+  </si>
+  <si>
+    <t>https://github.com/riscv/riscv-code-size-reduction/tree/main/Zc-specification</t>
+  </si>
+  <si>
+    <t>Zc specification</t>
+  </si>
+  <si>
+    <t>cd13c6b17ccb7e1b8fc8b69e76179b339bcc2b32</t>
+  </si>
+  <si>
+    <t>Zc cd13c6</t>
+  </si>
+  <si>
+    <t>Verify that all variations of these instructions decode as illegal 
+Cross check with instructions used in Zcmp/t</t>
+  </si>
+  <si>
+    <t>Verify illegal if Zbb is not configured</t>
+  </si>
+  <si>
+    <t>Verify all possible variations of uimm
+Note that this also includes illegal values</t>
+  </si>
+  <si>
+    <t>Verify exception behaviour, partially completed state shall match ISS: when a multi-operation instruction is stopped by an exception, state can have changed. Verify against ISS.
+Note: 40s implementation follows the example sequence in the Zc spec. ISS's should match this. (the order might change)
+Coverage note: cross between possible register lists and exception arriving between/at all sub-operations would be optimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zcmt
+Note: Deprioritize as this is furthest from ratification
+</t>
+  </si>
+  <si>
+    <t>Verify all table jump-related fetches are checked by PMP/PMA. Specifically break/follow the rules for both systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zcmb
+Note: Deprioritize as this is furthest from ratification
+</t>
+  </si>
+  <si>
+    <t>csr stateen bit 2 controls user mode access, if bit is not set, cm.jt and cm.jalt should decode as illegal.
+Access also controlled with smstateen, illegal if not enabled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify instruction with watchpoint triggers on data address </t>
+  </si>
+  <si>
+    <t>Zcb
+Note: For instructions with an uncompressed equivalent, check with design which are decoded to the 32b equivalent. For all others, consider a more thorough verification of the instruction, with regards to input values etc.</t>
   </si>
 </sst>
 </file>
@@ -465,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -524,16 +560,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,7 +581,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,12 +971,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ140"/>
+  <dimension ref="A1:AMF146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.4"/>
@@ -944,9 +989,9 @@
     <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5546875" style="1" customWidth="1"/>
-    <col min="10" max="1023" width="17" style="1"/>
-    <col min="1024" max="1024" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="50" style="1" customWidth="1"/>
+    <col min="10" max="1019" width="17" style="1"/>
+    <col min="1020" max="1020" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="28.2">
@@ -978,24 +1023,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A2" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>37</v>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="55.2">
+      <c r="A2" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>22</v>
@@ -1006,16 +1051,16 @@
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A3" s="28"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>23</v>
@@ -1029,880 +1074,876 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A4" s="28"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A5" s="29"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A6" s="29"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A7" s="29"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A8" s="29"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A9" s="29"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A10" s="29"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D10" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A11" s="29"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A12" s="29"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A13" s="29"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A14" s="29"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A15" s="29"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A16" s="29"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A17" s="29"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A18" s="29"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A19" s="29"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A20" s="29"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A21" s="29"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D22" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E22" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A23" s="29"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A24" s="29"/>
+      <c r="B24" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A25" s="29"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A26" s="29"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A27" s="29"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A28" s="29"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A29" s="29"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A30" s="29"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A31" s="29"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A32" s="29"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A33" s="29"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A34" s="29"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A35" s="29"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A36" s="29"/>
+      <c r="B36" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A37" s="29"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A5" s="28"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A6" s="28"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="F37" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A38" s="29"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A39" s="29"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A40" s="29"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A41" s="29"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A42" s="29"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A43" s="29"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A7" s="28"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A8" s="28"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A9" s="28"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A10" s="28"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A11" s="28"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A12" s="28"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A13" s="28"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A14" s="28"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A15" s="28"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A16" s="28"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A17" s="28"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A18" s="28"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A19" s="28"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A20" s="28"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A21" s="28"/>
-      <c r="B21" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A22" s="28"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A23" s="28"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A24" s="28"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A25" s="28"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A26" s="28"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A27" s="28"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A28" s="28"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A29" s="28"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A30" s="28"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A31" s="28"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A32" s="28"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A33" s="28"/>
-      <c r="B33" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A34" s="28"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A35" s="28"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="19" t="s">
+      <c r="F43" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A44" s="29"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H44" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" ht="138">
-      <c r="A36" s="28"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" ht="193.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A38" s="28"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A39" s="28"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A40" s="28"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" ht="138">
-      <c r="A41" s="28"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" ht="193.2">
-      <c r="A42" s="28"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A43" s="28"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A44" s="28"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>15</v>
-      </c>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A45" s="28"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G45" s="19" t="s">
         <v>19</v>
@@ -1913,12 +1954,12 @@
       <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" ht="138">
-      <c r="A46" s="28"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="20" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>18</v>
@@ -1932,15 +1973,15 @@
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" ht="193.2">
-      <c r="A47" s="28"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="20" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>22</v>
@@ -1950,20 +1991,20 @@
       </c>
       <c r="I47" s="12"/>
     </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A48" s="28"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>85</v>
+    <row r="48" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A48" s="29"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G48" s="19" t="s">
         <v>22</v>
@@ -1973,16 +2014,16 @@
       </c>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A49" s="28"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
+    <row r="49" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A49" s="29"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="16" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G49" s="19" t="s">
         <v>22</v>
@@ -1992,16 +2033,16 @@
       </c>
       <c r="I49" s="12"/>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
-      <c r="A50" s="28"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
+    <row r="50" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A50" s="29"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G50" s="19" t="s">
         <v>19</v>
@@ -2011,13 +2052,13 @@
       </c>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
-      <c r="A51" s="28"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+    <row r="51" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A51" s="29"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
       <c r="E51" s="20" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>18</v>
@@ -2030,16 +2071,16 @@
       </c>
       <c r="I51" s="12"/>
     </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
-      <c r="A52" s="28"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+    <row r="52" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A52" s="29"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="20" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>22</v>
@@ -2049,20 +2090,20 @@
       </c>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A53" s="28"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>106</v>
+    <row r="53" spans="1:9" s="3" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A53" s="29"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G53" s="19" t="s">
         <v>22</v>
@@ -2072,262 +2113,258 @@
       </c>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A54" s="28"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="19" t="s">
-        <v>111</v>
+    <row r="54" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A54" s="29"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G54" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A55" s="29"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G55" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="18" t="s">
+      <c r="H55" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I54" s="12"/>
-    </row>
-    <row r="55" spans="1:9" s="3" customFormat="1" ht="138">
-      <c r="A55" s="28"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F55" s="20" t="s">
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A56" s="29"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F56" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="22" t="s">
+      <c r="G56" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I55" s="12"/>
-    </row>
-    <row r="56" spans="1:9" s="3" customFormat="1" ht="193.2">
-      <c r="A56" s="28"/>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="22" t="s">
-        <v>15</v>
-      </c>
       <c r="I56" s="12"/>
     </row>
-    <row r="57" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A57" s="28"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="18" t="s">
+    <row r="57" spans="1:9" s="3" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A57" s="29"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="22" t="s">
         <v>15</v>
       </c>
       <c r="I57" s="12"/>
     </row>
-    <row r="58" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A58" s="28"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="26"/>
+    <row r="58" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A58" s="29"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>76</v>
+      </c>
       <c r="E58" s="19" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G58" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A59" s="29"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G59" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H58" s="18" t="s">
+      <c r="H59" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I58" s="12"/>
-    </row>
-    <row r="59" spans="1:9" s="3" customFormat="1" ht="138">
-      <c r="A59" s="28"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F59" s="20" t="s">
+      <c r="I59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A60" s="29"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H59" s="22" t="s">
+      <c r="G60" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="12"/>
-    </row>
-    <row r="60" spans="1:9" s="3" customFormat="1" ht="193.2">
-      <c r="A60" s="28"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G60" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H60" s="22" t="s">
-        <v>15</v>
-      </c>
       <c r="I60" s="12"/>
     </row>
-    <row r="61" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A61" s="28"/>
-      <c r="B61" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="18" t="s">
+    <row r="61" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A61" s="29"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="22" t="s">
         <v>15</v>
       </c>
       <c r="I61" s="12"/>
     </row>
-    <row r="62" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A62" s="28"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="26"/>
+    <row r="62" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A62" s="29"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>77</v>
+      </c>
       <c r="E62" s="19" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I62" s="12"/>
     </row>
-    <row r="63" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A63" s="28"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>89</v>
-      </c>
+    <row r="63" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A63" s="29"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="19" t="s">
         <v>99</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I63" s="12"/>
     </row>
-    <row r="64" spans="1:9" s="3" customFormat="1" ht="82.8">
-      <c r="A64" s="28"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="24"/>
+    <row r="64" spans="1:9" s="3" customFormat="1" ht="138">
+      <c r="A64" s="29"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="25"/>
       <c r="D64" s="26"/>
-      <c r="E64" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H64" s="18" t="s">
-        <v>12</v>
+      <c r="E64" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="I64" s="12"/>
     </row>
-    <row r="65" spans="1:9" s="3" customFormat="1" ht="41.4">
-      <c r="A65" s="28"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="24" t="s">
+    <row r="65" spans="1:9" s="3" customFormat="1" ht="193.2">
+      <c r="A65" s="29"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>12</v>
+      <c r="F65" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="I65" s="12"/>
     </row>
-    <row r="66" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A66" s="28"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="26"/>
+    <row r="66" spans="1:9" s="3" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A66" s="29"/>
+      <c r="B66" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>78</v>
+      </c>
       <c r="E66" s="19" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G66" s="19" t="s">
         <v>22</v>
@@ -2337,101 +2374,157 @@
       </c>
       <c r="I66" s="12"/>
     </row>
-    <row r="67" spans="1:9" s="3" customFormat="1" ht="27.6">
-      <c r="A67" s="28"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="26"/>
+    <row r="67" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A67" s="29"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="32"/>
       <c r="E67" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G67" s="19" t="s">
         <v>19</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="1:9" s="3" customFormat="1">
-      <c r="A68" s="4"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="12"/>
+    <row r="68" spans="1:9" s="3" customFormat="1" ht="41.4">
+      <c r="A68" s="29"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F68" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="I68" s="12"/>
     </row>
-    <row r="69" spans="1:9" s="3" customFormat="1">
-      <c r="A69" s="4"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-    </row>
-    <row r="70" spans="1:9" s="3" customFormat="1">
-      <c r="A70" s="4"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-    </row>
-    <row r="71" spans="1:9" s="3" customFormat="1">
-      <c r="A71" s="4"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-    </row>
-    <row r="72" spans="1:9" s="3" customFormat="1">
-      <c r="A72" s="4"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-    </row>
-    <row r="73" spans="1:9" s="3" customFormat="1">
-      <c r="A73" s="4"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
+    <row r="69" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A69" s="29"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="12"/>
+    </row>
+    <row r="70" spans="1:9" s="3" customFormat="1" ht="82.8">
+      <c r="A70" s="29"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" s="12"/>
+    </row>
+    <row r="71" spans="1:9" s="3" customFormat="1" ht="69">
+      <c r="A71" s="29"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="12"/>
+    </row>
+    <row r="72" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A72" s="29"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="12"/>
+    </row>
+    <row r="73" spans="1:9" s="3" customFormat="1" ht="27.6">
+      <c r="A73" s="29"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I73" s="12"/>
     </row>
     <row r="74" spans="1:9" s="3" customFormat="1">
       <c r="A74" s="4"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
     </row>
     <row r="75" spans="1:9" s="3" customFormat="1">
       <c r="A75" s="4"/>
@@ -2727,8 +2820,8 @@
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
     </row>
     <row r="102" spans="1:9" s="3" customFormat="1">
       <c r="A102" s="4"/>
@@ -2738,8 +2831,8 @@
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
+      <c r="H102" s="11"/>
+      <c r="I102" s="11"/>
     </row>
     <row r="103" spans="1:9" s="3" customFormat="1">
       <c r="A103" s="4"/>
@@ -2749,8 +2842,8 @@
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="11"/>
     </row>
     <row r="104" spans="1:9" s="3" customFormat="1">
       <c r="A104" s="4"/>
@@ -2760,8 +2853,8 @@
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
     </row>
     <row r="105" spans="1:9" s="3" customFormat="1">
       <c r="A105" s="4"/>
@@ -2771,8 +2864,8 @@
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
     </row>
     <row r="106" spans="1:9" s="3" customFormat="1">
       <c r="A106" s="4"/>
@@ -2782,8 +2875,8 @@
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="11"/>
     </row>
     <row r="107" spans="1:9" s="3" customFormat="1">
       <c r="A107" s="4"/>
@@ -3148,52 +3241,119 @@
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="1:9" s="6" customFormat="1">
-      <c r="A140" s="27" t="s">
+    <row r="140" spans="1:9" s="3" customFormat="1">
+      <c r="A140" s="4"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+    </row>
+    <row r="141" spans="1:9" s="3" customFormat="1">
+      <c r="A141" s="4"/>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+    </row>
+    <row r="142" spans="1:9" s="3" customFormat="1">
+      <c r="A142" s="4"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+    </row>
+    <row r="143" spans="1:9" s="3" customFormat="1">
+      <c r="A143" s="4"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+    </row>
+    <row r="144" spans="1:9" s="3" customFormat="1">
+      <c r="A144" s="4"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+    </row>
+    <row r="145" spans="1:9" s="3" customFormat="1">
+      <c r="A145" s="4"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+    </row>
+    <row r="146" spans="1:9" s="6" customFormat="1">
+      <c r="A146" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B140" s="27"/>
-      <c r="C140" s="27"/>
-      <c r="D140" s="27"/>
-      <c r="E140" s="27"/>
-      <c r="F140" s="27"/>
-      <c r="G140" s="27"/>
-      <c r="H140" s="27"/>
-      <c r="I140" s="27"/>
+      <c r="B146" s="28"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="28"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="28"/>
+      <c r="G146" s="28"/>
+      <c r="H146" s="28"/>
+      <c r="I146" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="63">
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B36:B63"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="D36:D41"/>
     <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A140:I140"/>
-    <mergeCell ref="A2:A67"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="A146:I146"/>
+    <mergeCell ref="A2:A73"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B20"/>
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="B61:B67"/>
+    <mergeCell ref="B4:B23"/>
+    <mergeCell ref="B24:B35"/>
+    <mergeCell ref="B66:B73"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D8:D9"/>
@@ -3204,24 +3364,27 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="B33:B58"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3235,7 +3398,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H139</xm:sqref>
+          <xm:sqref>H69:H145 H2:H67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -3244,7 +3407,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G2:G139</xm:sqref>
+          <xm:sqref>G69:G145 G2:G67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -3253,7 +3416,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F139</xm:sqref>
+          <xm:sqref>F69:F145 F2:F67</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3313,7 +3476,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -3373,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -3404,33 +3567,47 @@
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>32</v>
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="10" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>36</v>
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>